<commit_message>
Forgot to push changes from Wahl's feedback
</commit_message>
<xml_diff>
--- a/ExampleResults.xlsx
+++ b/ExampleResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\git\DUBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D023A882-51B0-4C2A-9ECA-BECE7E787DC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABE889E-B7F0-4B2F-92AF-C36C986F5BAE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9FC16A22-990D-4BAB-9E2C-FCAEF63428DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FC16A22-990D-4BAB-9E2C-FCAEF63428DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>File Name</t>
   </si>
@@ -593,15 +593,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926923B2-1397-46A0-AE74-8DE000CDA604}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,10 +622,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>47</v>
@@ -648,10 +648,10 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -671,10 +671,10 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -693,23 +693,17 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>45</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5">
         <v>5</v>
       </c>
@@ -719,23 +713,17 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
         <v>45</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
       </c>
       <c r="H5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
       <c r="C6">
         <v>5</v>
       </c>
@@ -746,10 +734,10 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -768,23 +756,17 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>45</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
       <c r="C8">
         <v>5</v>
       </c>
@@ -795,10 +777,10 @@
         <v>3</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -818,10 +800,10 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" t="s">
         <v>51</v>
@@ -844,10 +826,10 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -867,10 +849,10 @@
         <v>3</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -890,10 +872,10 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -913,10 +895,10 @@
         <v>2</v>
       </c>
       <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>4</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -936,10 +918,10 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -958,23 +940,17 @@
       <c r="E16">
         <v>3</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>45</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
       </c>
       <c r="H16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
       <c r="C17">
         <v>20</v>
       </c>
@@ -985,10 +961,10 @@
         <v>3</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1007,20 +983,14 @@
       <c r="E18">
         <v>4</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
         <v>45</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
       <c r="C19">
         <v>20</v>
       </c>
@@ -1031,10 +1001,10 @@
         <v>4</v>
       </c>
       <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
         <v>9</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
       </c>
       <c r="H19" t="s">
         <v>53</v>
@@ -1056,23 +1026,17 @@
       <c r="E20">
         <v>4</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>45</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
       </c>
       <c r="H20" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
       <c r="C21">
         <v>20</v>
       </c>
@@ -1083,10 +1047,10 @@
         <v>4</v>
       </c>
       <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
         <v>12</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
       </c>
       <c r="H21" t="s">
         <v>55</v>
@@ -1108,23 +1072,17 @@
       <c r="E22">
         <v>3</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>45</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
       </c>
       <c r="H22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
       <c r="C23">
         <v>20</v>
       </c>
@@ -1135,10 +1093,10 @@
         <v>3</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H23" t="s">
         <v>57</v>
@@ -1161,10 +1119,10 @@
         <v>4</v>
       </c>
       <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
         <v>9</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1184,10 +1142,10 @@
         <v>4</v>
       </c>
       <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
         <v>12</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
       </c>
       <c r="H25" t="s">
         <v>58</v>
@@ -1210,10 +1168,10 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H26" t="s">
         <v>59</v>
@@ -1236,10 +1194,10 @@
         <v>4</v>
       </c>
       <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
         <v>9</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1259,10 +1217,10 @@
         <v>4</v>
       </c>
       <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
         <v>12</v>
-      </c>
-      <c r="G28">
-        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1282,10 +1240,10 @@
         <v>2</v>
       </c>
       <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
         <v>4</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
       </c>
       <c r="H29" t="s">
         <v>60</v>
@@ -1308,10 +1266,10 @@
         <v>3</v>
       </c>
       <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
         <v>7</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
       </c>
       <c r="H30" t="s">
         <v>61</v>
@@ -1334,10 +1292,10 @@
         <v>3</v>
       </c>
       <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
         <v>9</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
       </c>
       <c r="H31" t="s">
         <v>62</v>
@@ -1359,23 +1317,17 @@
       <c r="E32">
         <v>3</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
         <v>45</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
       </c>
       <c r="H32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
       <c r="C33">
         <v>20</v>
       </c>
@@ -1386,10 +1338,10 @@
         <v>3</v>
       </c>
       <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
         <v>9</v>
-      </c>
-      <c r="G33">
-        <v>2</v>
       </c>
       <c r="H33" t="s">
         <v>63</v>
@@ -1412,10 +1364,10 @@
         <v>2</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H34" t="s">
         <v>65</v>
@@ -1438,10 +1390,10 @@
         <v>4</v>
       </c>
       <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
         <v>8</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,10 +1413,10 @@
         <v>2</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" t="s">
         <v>66</v>
@@ -1487,10 +1439,10 @@
         <v>4</v>
       </c>
       <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
         <v>4</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
       </c>
       <c r="H37" t="s">
         <v>68</v>
@@ -1512,11 +1464,11 @@
       <c r="E38">
         <v>8</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
         <v>45</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
       </c>
       <c r="H38" t="s">
         <v>67</v>
@@ -1539,10 +1491,10 @@
         <v>2</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H39" t="s">
         <v>69</v>

</xml_diff>